<commit_message>
Acc. tracer data to ssf
</commit_message>
<xml_diff>
--- a/data/observations/obs_head_per_layer.xlsx
+++ b/data/observations/obs_head_per_layer.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="2" r:id="rId1"/>
@@ -96,12 +96,6 @@
     <t>NI1606-3</t>
   </si>
   <si>
-    <t>NI1605b-1</t>
-  </si>
-  <si>
-    <t>NI1605b-3</t>
-  </si>
-  <si>
     <t>NI1604-1</t>
   </si>
   <si>
@@ -261,12 +255,6 @@
     <t>NI1403-2</t>
   </si>
   <si>
-    <t>NI1402b-1</t>
-  </si>
-  <si>
-    <t>NI1402b-2</t>
-  </si>
-  <si>
     <t>NI1401-1</t>
   </si>
   <si>
@@ -463,6 +451,18 @@
   </si>
   <si>
     <t>B9-5</t>
+  </si>
+  <si>
+    <t>NI1402-2</t>
+  </si>
+  <si>
+    <t>NI1402-1</t>
+  </si>
+  <si>
+    <t>NI1605-1</t>
+  </si>
+  <si>
+    <t>NI1605-3</t>
   </si>
 </sst>
 </file>
@@ -782,19 +782,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -803,12 +803,12 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B2">
         <v>426918.37400000001</v>
@@ -820,9 +820,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3">
         <v>427074.70942299999</v>
@@ -834,9 +834,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B4">
         <v>427448.18850500003</v>
@@ -848,9 +848,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>427409.54730099998</v>
@@ -862,9 +862,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B6">
         <v>427384.17204400001</v>
@@ -876,9 +876,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B7">
         <v>427448.93046300003</v>
@@ -890,9 +890,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B8">
         <v>427455.40708400001</v>
@@ -904,9 +904,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B9">
         <v>427375.04528600001</v>
@@ -918,9 +918,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B10">
         <v>427405.59223499999</v>
@@ -932,9 +932,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B11">
         <v>427230.095133</v>
@@ -946,9 +946,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B12">
         <v>427461.85729999997</v>
@@ -960,9 +960,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <v>427451.795231</v>
@@ -974,9 +974,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B14">
         <v>427470.63105600001</v>
@@ -988,9 +988,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B15">
         <v>427471.152459</v>
@@ -1002,9 +1002,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16">
         <v>427437.28213900002</v>
@@ -1016,9 +1016,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17">
         <v>427428.46884500002</v>
@@ -1030,9 +1030,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>427449.97970800003</v>
@@ -1044,9 +1044,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>427463.33470299997</v>
@@ -1058,9 +1058,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20">
         <v>427464.67415799998</v>
@@ -1072,9 +1072,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>427463.52186600002</v>
@@ -1086,9 +1086,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>427456.07263200002</v>
@@ -1100,9 +1100,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>427363.30535500002</v>
@@ -1114,9 +1114,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24">
         <v>427443.730048</v>
@@ -1128,9 +1128,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25">
         <v>427449.771824</v>
@@ -1142,9 +1142,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>427453.49740699999</v>
@@ -1156,9 +1156,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>427443.16329699999</v>
@@ -1170,9 +1170,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>427445.95748500002</v>
@@ -1184,9 +1184,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B29">
         <v>427391.988166</v>
@@ -1198,9 +1198,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B30">
         <v>427385.27214800002</v>
@@ -1212,9 +1212,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B31">
         <v>427316.29342100001</v>
@@ -1226,9 +1226,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B32">
         <v>427294.94666100002</v>
@@ -1240,9 +1240,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B33">
         <v>427166.67072200001</v>
@@ -1254,9 +1254,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>427409.62389599998</v>
@@ -1268,9 +1268,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35">
         <v>427348.77541900001</v>
@@ -1282,9 +1282,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B36">
         <v>427358.29147300002</v>
@@ -1296,9 +1296,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="B37">
         <v>427474.83270700002</v>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1366,9 +1366,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B42">
         <v>427398.293687</v>
@@ -1380,9 +1380,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B43">
         <v>427404.40658499999</v>
@@ -1394,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1408,9 +1408,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B45">
         <v>427359.14739400003</v>
@@ -1422,9 +1422,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B46">
         <v>427397.79165600002</v>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1464,611 +1464,611 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B49">
+        <v>427416.82571</v>
+      </c>
+      <c r="C49">
+        <v>6654931.4033899996</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50">
         <v>427199.387766</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>6654953.6541600004</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51">
         <v>427206.01863000001</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>6654952.8338099997</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>119</v>
-      </c>
-      <c r="B51">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52">
         <v>427211.63491899997</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>6654950.92655</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53">
+        <v>427218.57246400003</v>
+      </c>
+      <c r="C53">
+        <v>6654949.0793199996</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54">
+        <v>426918.37400000001</v>
+      </c>
+      <c r="C54">
+        <v>6654803.2980000004</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55">
+        <v>427074.70942299999</v>
+      </c>
+      <c r="C55">
+        <v>6654805.1742099999</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56">
+        <v>427464.68924600002</v>
+      </c>
+      <c r="C56">
+        <v>6655155.0027599996</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57">
+        <v>427474.42482399999</v>
+      </c>
+      <c r="C57">
+        <v>6655148.0094600003</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58">
+        <v>427480.544406</v>
+      </c>
+      <c r="C58">
+        <v>6655184.8646900002</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59">
+        <v>427445.73171299999</v>
+      </c>
+      <c r="C59">
+        <v>6655165.4479799997</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60">
+        <v>427454.97677200002</v>
+      </c>
+      <c r="C60">
+        <v>6655155.6970300004</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61">
+        <v>427384.17204400001</v>
+      </c>
+      <c r="C61">
+        <v>6655037.1886999998</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62">
+        <v>427448.93046300003</v>
+      </c>
+      <c r="C62">
+        <v>6655144.2890999997</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63">
+        <v>427464.31650100002</v>
+      </c>
+      <c r="C63">
+        <v>6655164.6224400001</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>130</v>
+      </c>
+      <c r="B64">
+        <v>427447.84926599998</v>
+      </c>
+      <c r="C64">
+        <v>6655002.2449700003</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65">
+        <v>427448.60130400001</v>
+      </c>
+      <c r="C65">
+        <v>6654991.7577499999</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66">
+        <v>427461.17045699997</v>
+      </c>
+      <c r="C66">
+        <v>6654998.4210900003</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67">
+        <v>427162.88967599999</v>
+      </c>
+      <c r="C67">
+        <v>6654757.2354899999</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>121</v>
       </c>
-      <c r="B52">
-        <v>427218.57246400003</v>
-      </c>
-      <c r="C52">
-        <v>6654949.0793199996</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>146</v>
-      </c>
-      <c r="B53">
-        <v>426918.37400000001</v>
-      </c>
-      <c r="C53">
-        <v>6654803.2980000004</v>
-      </c>
-      <c r="D53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>107</v>
-      </c>
-      <c r="B54">
-        <v>427074.70942299999</v>
-      </c>
-      <c r="C54">
-        <v>6654805.1742099999</v>
-      </c>
-      <c r="D54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>127</v>
-      </c>
-      <c r="B55">
-        <v>427464.68924600002</v>
-      </c>
-      <c r="C55">
-        <v>6655155.0027599996</v>
-      </c>
-      <c r="D55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56">
-        <v>427474.42482399999</v>
-      </c>
-      <c r="C56">
-        <v>6655148.0094600003</v>
-      </c>
-      <c r="D56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>129</v>
-      </c>
-      <c r="B57">
-        <v>427480.544406</v>
-      </c>
-      <c r="C57">
-        <v>6655184.8646900002</v>
-      </c>
-      <c r="D57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>130</v>
-      </c>
-      <c r="B58">
-        <v>427445.73171299999</v>
-      </c>
-      <c r="C58">
-        <v>6655165.4479799997</v>
-      </c>
-      <c r="D58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59">
-        <v>427454.97677200002</v>
-      </c>
-      <c r="C59">
-        <v>6655155.6970300004</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60">
-        <v>427384.17204400001</v>
-      </c>
-      <c r="C60">
-        <v>6655037.1886999998</v>
-      </c>
-      <c r="D60">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>96</v>
-      </c>
-      <c r="B61">
-        <v>427448.93046300003</v>
-      </c>
-      <c r="C61">
-        <v>6655144.2890999997</v>
-      </c>
-      <c r="D61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>131</v>
-      </c>
-      <c r="B62">
-        <v>427464.31650100002</v>
-      </c>
-      <c r="C62">
-        <v>6655164.6224400001</v>
-      </c>
-      <c r="D62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>134</v>
-      </c>
-      <c r="B63">
-        <v>427447.84926599998</v>
-      </c>
-      <c r="C63">
-        <v>6655002.2449700003</v>
-      </c>
-      <c r="D63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>135</v>
-      </c>
-      <c r="B64">
-        <v>427448.60130400001</v>
-      </c>
-      <c r="C64">
-        <v>6654991.7577499999</v>
-      </c>
-      <c r="D64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>136</v>
-      </c>
-      <c r="B65">
-        <v>427461.17045699997</v>
-      </c>
-      <c r="C65">
-        <v>6654998.4210900003</v>
-      </c>
-      <c r="D65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>90</v>
-      </c>
-      <c r="B66">
-        <v>427162.88967599999</v>
-      </c>
-      <c r="C66">
-        <v>6654757.2354899999</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>125</v>
-      </c>
-      <c r="B67">
+      <c r="B68">
         <v>427230.095133</v>
       </c>
-      <c r="C67">
+      <c r="C68">
         <v>6654957.8994800001</v>
       </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>88</v>
-      </c>
-      <c r="B68">
+      <c r="D68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69">
         <v>427461.85729999997</v>
       </c>
-      <c r="C68">
+      <c r="C69">
         <v>6655153.3641299997</v>
       </c>
-      <c r="D68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>85</v>
-      </c>
-      <c r="B69">
+      <c r="D69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70">
         <v>427451.795231</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>6655150.5926099997</v>
       </c>
-      <c r="D69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70">
+      <c r="D70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71">
         <v>427454.58941900003</v>
       </c>
-      <c r="C70">
+      <c r="C71">
         <v>6655141.5299500003</v>
       </c>
-      <c r="D70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71">
+      <c r="D71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72">
         <v>427451.88591100002</v>
       </c>
-      <c r="C71">
+      <c r="C72">
         <v>6655154.5902399998</v>
       </c>
-      <c r="D71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72">
+      <c r="D72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
         <v>427459.94916800002</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>6655157.4070899999</v>
       </c>
-      <c r="D72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>71</v>
-      </c>
-      <c r="B73">
+      <c r="D73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74">
         <v>427437.28213900002</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>6655127.9236500002</v>
       </c>
-      <c r="D73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>68</v>
-      </c>
-      <c r="B74">
+      <c r="D74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75">
         <v>427428.46884500002</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <v>6655136.1229299996</v>
       </c>
-      <c r="D74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>65</v>
-      </c>
-      <c r="B75">
+      <c r="D75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76">
         <v>427449.97970800003</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <v>6655114.6366699999</v>
       </c>
-      <c r="D75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>62</v>
-      </c>
-      <c r="B76">
+      <c r="D76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>60</v>
+      </c>
+      <c r="B77">
         <v>427463.33470299997</v>
       </c>
-      <c r="C76">
+      <c r="C77">
         <v>6655130.3324499996</v>
       </c>
-      <c r="D76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>59</v>
-      </c>
-      <c r="B77">
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>57</v>
+      </c>
+      <c r="B78">
         <v>427464.67415799998</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>6655145.3008700004</v>
       </c>
-      <c r="D77">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>54</v>
-      </c>
-      <c r="B78">
+      <c r="D78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79">
         <v>427456.07263200002</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>6654986.50868</v>
       </c>
-      <c r="D78">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>51</v>
-      </c>
-      <c r="B79">
+      <c r="D79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B80">
         <v>427363.30535500002</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>6655084.6052799998</v>
       </c>
-      <c r="D79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>42</v>
-      </c>
-      <c r="B80">
+      <c r="D80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>40</v>
+      </c>
+      <c r="B81">
         <v>427443.16329699999</v>
       </c>
-      <c r="C80">
+      <c r="C81">
         <v>6655166.7871399997</v>
       </c>
-      <c r="D80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>39</v>
-      </c>
-      <c r="B81">
+      <c r="D81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82">
         <v>427445.95748500002</v>
       </c>
-      <c r="C81">
+      <c r="C82">
         <v>6655157.7244699998</v>
       </c>
-      <c r="D81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>36</v>
-      </c>
-      <c r="B82">
-        <v>427419.01886399998</v>
-      </c>
-      <c r="C82">
-        <v>6655160.3353700005</v>
-      </c>
       <c r="D82">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>34</v>
       </c>
       <c r="B83">
+        <v>427419.01886399998</v>
+      </c>
+      <c r="C83">
+        <v>6655160.3353700005</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84">
         <v>427409.62389599998</v>
       </c>
-      <c r="C83">
+      <c r="C84">
         <v>6654966.5639599999</v>
       </c>
-      <c r="D83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>27</v>
-      </c>
-      <c r="B84">
+      <c r="D84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>25</v>
+      </c>
+      <c r="B85">
         <v>427459.27487700002</v>
       </c>
-      <c r="C84">
+      <c r="C85">
         <v>6654995.4353299998</v>
       </c>
-      <c r="D84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="D85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>23</v>
       </c>
-      <c r="B85">
+      <c r="B86">
         <v>427309.979934</v>
       </c>
-      <c r="C85">
+      <c r="C86">
         <v>6654937.8266599998</v>
       </c>
-      <c r="D85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="D86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>20</v>
       </c>
-      <c r="B86">
+      <c r="B87">
         <v>427397.49695300002</v>
       </c>
-      <c r="C86">
+      <c r="C87">
         <v>6654916.8430199996</v>
       </c>
-      <c r="D86">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="D87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>17</v>
       </c>
-      <c r="B87">
+      <c r="B88">
         <v>427394.22670100001</v>
       </c>
-      <c r="C87">
+      <c r="C88">
         <v>6654904.9181599999</v>
       </c>
-      <c r="D87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="D88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>109</v>
+      </c>
+      <c r="B89">
+        <v>427397.79165600002</v>
+      </c>
+      <c r="C89">
+        <v>6654929.8353000004</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>427250.03822699998</v>
+      </c>
+      <c r="C90">
+        <v>6654940.1862300001</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>110</v>
+      </c>
+      <c r="B91">
+        <v>427488.90997899999</v>
+      </c>
+      <c r="C91">
+        <v>6655046.4589799996</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>113</v>
-      </c>
-      <c r="B88">
-        <v>427397.79165600002</v>
-      </c>
-      <c r="C88">
-        <v>6654929.8353000004</v>
-      </c>
-      <c r="D88">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89">
-        <v>427250.03822699998</v>
-      </c>
-      <c r="C89">
-        <v>6654940.1862300001</v>
-      </c>
-      <c r="D89">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>114</v>
-      </c>
-      <c r="B90">
-        <v>427488.90997899999</v>
-      </c>
-      <c r="C90">
-        <v>6655046.4589799996</v>
-      </c>
-      <c r="D90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>115</v>
-      </c>
-      <c r="B91">
-        <v>427416.82571</v>
-      </c>
-      <c r="C91">
-        <v>6654931.4033899996</v>
-      </c>
-      <c r="D91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>117</v>
       </c>
       <c r="B92">
         <v>427199.387766</v>
@@ -2080,9 +2080,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B93">
         <v>427211.63491899997</v>
@@ -2094,9 +2094,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B94">
         <v>427218.57246400003</v>
@@ -2108,9 +2108,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B95">
         <v>426918.37400000001</v>
@@ -2122,9 +2122,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B96">
         <v>427074.70942299999</v>
@@ -2136,9 +2136,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B97">
         <v>427409.54730099998</v>
@@ -2150,9 +2150,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B98">
         <v>427473.89030299999</v>
@@ -2164,9 +2164,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B99">
         <v>427454.97677200002</v>
@@ -2178,9 +2178,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B100">
         <v>427448.93046300003</v>
@@ -2192,9 +2192,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B101">
         <v>427384.17204400001</v>
@@ -2206,9 +2206,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B102">
         <v>427353.18437899998</v>
@@ -2220,9 +2220,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B103">
         <v>427436.22735900001</v>
@@ -2234,9 +2234,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B104">
         <v>427473.82857299998</v>
@@ -2248,9 +2248,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B105">
         <v>427162.88967599999</v>
@@ -2262,9 +2262,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B106">
         <v>427461.85729999997</v>
@@ -2276,9 +2276,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B107">
         <v>427451.795231</v>
@@ -2290,9 +2290,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B108">
         <v>427454.58941900003</v>
@@ -2304,9 +2304,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="B109">
         <v>427451.88591100002</v>
@@ -2318,9 +2318,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B110">
         <v>427470.63105600001</v>
@@ -2332,9 +2332,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B111">
         <v>427459.94916800002</v>
@@ -2346,9 +2346,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B112">
         <v>427471.152459</v>
@@ -2360,9 +2360,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B113">
         <v>427448.77434300003</v>
@@ -2374,9 +2374,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B114">
         <v>427437.28213900002</v>
@@ -2388,9 +2388,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B115">
         <v>427428.46884500002</v>
@@ -2402,9 +2402,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B116">
         <v>427449.97970800003</v>
@@ -2416,9 +2416,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B117">
         <v>427463.33470299997</v>
@@ -2430,9 +2430,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B118">
         <v>427464.67415799998</v>
@@ -2444,9 +2444,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B119">
         <v>427463.52186600002</v>
@@ -2458,9 +2458,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B120">
         <v>427456.07263200002</v>
@@ -2472,9 +2472,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B121">
         <v>427363.30535500002</v>
@@ -2486,9 +2486,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B122">
         <v>427443.730048</v>
@@ -2500,9 +2500,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B123">
         <v>427449.771824</v>
@@ -2514,9 +2514,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B124">
         <v>427453.49740699999</v>
@@ -2528,9 +2528,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B125">
         <v>427443.16329699999</v>
@@ -2542,9 +2542,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B126">
         <v>427445.95748500002</v>
@@ -2556,9 +2556,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B127">
         <v>427419.01886399998</v>
@@ -2570,9 +2570,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B128">
         <v>427409.62389599998</v>
@@ -2584,9 +2584,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B129">
         <v>427348.77541900001</v>
@@ -2598,9 +2598,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B130">
         <v>427358.29147300002</v>
@@ -2612,9 +2612,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B131">
         <v>427459.27487700002</v>
@@ -2626,9 +2626,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>26</v>
+        <v>147</v>
       </c>
       <c r="B132">
         <v>427474.83270700002</v>
@@ -2640,7 +2640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>24</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>21</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>18</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>15</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>13</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>10</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -2752,9 +2752,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B141">
         <v>427215.44438599999</v>
@@ -2766,7 +2766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>6</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>4</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>3</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
New notebooks (obs & calib setup)
Notebooks aren't completed yet though...
</commit_message>
<xml_diff>
--- a/data/observations/obs_head_per_layer.xlsx
+++ b/data/observations/obs_head_per_layer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>POINT_X</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>NI1605-3</t>
+  </si>
+  <si>
+    <t>KB1-2</t>
   </si>
 </sst>
 </file>
@@ -780,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D145"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G85" sqref="G85"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,13 +1735,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="B68">
-        <v>427230.095133</v>
+        <v>427404.96500000003</v>
       </c>
       <c r="C68">
-        <v>6654957.8994800001</v>
+        <v>6654944.7280000001</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -1746,13 +1749,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="B69">
-        <v>427461.85729999997</v>
+        <v>427230.095133</v>
       </c>
       <c r="C69">
-        <v>6655153.3641299997</v>
+        <v>6654957.8994800001</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -1760,13 +1763,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B70">
-        <v>427451.795231</v>
+        <v>427461.85729999997</v>
       </c>
       <c r="C70">
-        <v>6655150.5926099997</v>
+        <v>6655153.3641299997</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -1774,13 +1777,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B71">
-        <v>427454.58941900003</v>
+        <v>427451.795231</v>
       </c>
       <c r="C71">
-        <v>6655141.5299500003</v>
+        <v>6655150.5926099997</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -1788,13 +1791,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="B72">
-        <v>427451.88591100002</v>
+        <v>427454.58941900003</v>
       </c>
       <c r="C72">
-        <v>6655154.5902399998</v>
+        <v>6655141.5299500003</v>
       </c>
       <c r="D72">
         <v>2</v>
@@ -1802,13 +1805,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="B73">
-        <v>427459.94916800002</v>
+        <v>427451.88591100002</v>
       </c>
       <c r="C73">
-        <v>6655157.4070899999</v>
+        <v>6655154.5902399998</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -1816,13 +1819,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B74">
-        <v>427437.28213900002</v>
+        <v>427459.94916800002</v>
       </c>
       <c r="C74">
-        <v>6655127.9236500002</v>
+        <v>6655157.4070899999</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -1830,13 +1833,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B75">
-        <v>427428.46884500002</v>
+        <v>427437.28213900002</v>
       </c>
       <c r="C75">
-        <v>6655136.1229299996</v>
+        <v>6655127.9236500002</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -1844,13 +1847,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B76">
-        <v>427449.97970800003</v>
+        <v>427428.46884500002</v>
       </c>
       <c r="C76">
-        <v>6655114.6366699999</v>
+        <v>6655136.1229299996</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -1858,13 +1861,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B77">
-        <v>427463.33470299997</v>
+        <v>427449.97970800003</v>
       </c>
       <c r="C77">
-        <v>6655130.3324499996</v>
+        <v>6655114.6366699999</v>
       </c>
       <c r="D77">
         <v>2</v>
@@ -1872,13 +1875,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B78">
-        <v>427464.67415799998</v>
+        <v>427463.33470299997</v>
       </c>
       <c r="C78">
-        <v>6655145.3008700004</v>
+        <v>6655130.3324499996</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -1886,13 +1889,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B79">
-        <v>427456.07263200002</v>
+        <v>427464.67415799998</v>
       </c>
       <c r="C79">
-        <v>6654986.50868</v>
+        <v>6655145.3008700004</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -1900,13 +1903,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B80">
-        <v>427363.30535500002</v>
+        <v>427456.07263200002</v>
       </c>
       <c r="C80">
-        <v>6655084.6052799998</v>
+        <v>6654986.50868</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -1914,13 +1917,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B81">
-        <v>427443.16329699999</v>
+        <v>427363.30535500002</v>
       </c>
       <c r="C81">
-        <v>6655166.7871399997</v>
+        <v>6655084.6052799998</v>
       </c>
       <c r="D81">
         <v>2</v>
@@ -1928,13 +1931,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B82">
-        <v>427445.95748500002</v>
+        <v>427443.16329699999</v>
       </c>
       <c r="C82">
-        <v>6655157.7244699998</v>
+        <v>6655166.7871399997</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -1942,13 +1945,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B83">
-        <v>427419.01886399998</v>
+        <v>427445.95748500002</v>
       </c>
       <c r="C83">
-        <v>6655160.3353700005</v>
+        <v>6655157.7244699998</v>
       </c>
       <c r="D83">
         <v>2</v>
@@ -1956,13 +1959,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B84">
-        <v>427409.62389599998</v>
+        <v>427419.01886399998</v>
       </c>
       <c r="C84">
-        <v>6654966.5639599999</v>
+        <v>6655160.3353700005</v>
       </c>
       <c r="D84">
         <v>2</v>
@@ -1970,13 +1973,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B85">
-        <v>427459.27487700002</v>
+        <v>427409.62389599998</v>
       </c>
       <c r="C85">
-        <v>6654995.4353299998</v>
+        <v>6654966.5639599999</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -1984,13 +1987,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B86">
-        <v>427309.979934</v>
+        <v>427459.27487700002</v>
       </c>
       <c r="C86">
-        <v>6654937.8266599998</v>
+        <v>6654995.4353299998</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -1998,13 +2001,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B87">
-        <v>427397.49695300002</v>
+        <v>427309.979934</v>
       </c>
       <c r="C87">
-        <v>6654916.8430199996</v>
+        <v>6654937.8266599998</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -2012,13 +2015,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B88">
-        <v>427394.22670100001</v>
+        <v>427397.49695300002</v>
       </c>
       <c r="C88">
-        <v>6654904.9181599999</v>
+        <v>6654916.8430199996</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -2026,13 +2029,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="B89">
-        <v>427397.79165600002</v>
+        <v>427394.22670100001</v>
       </c>
       <c r="C89">
-        <v>6654929.8353000004</v>
+        <v>6654904.9181599999</v>
       </c>
       <c r="D89">
         <v>2</v>
@@ -2040,13 +2043,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="B90">
-        <v>427250.03822699998</v>
+        <v>427397.79165600002</v>
       </c>
       <c r="C90">
-        <v>6654940.1862300001</v>
+        <v>6654929.8353000004</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -2054,13 +2057,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="B91">
-        <v>427488.90997899999</v>
+        <v>427250.03822699998</v>
       </c>
       <c r="C91">
-        <v>6655046.4589799996</v>
+        <v>6654940.1862300001</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -2068,13 +2071,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B92">
-        <v>427199.387766</v>
+        <v>427488.90997899999</v>
       </c>
       <c r="C92">
-        <v>6654953.6541600004</v>
+        <v>6655046.4589799996</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -2082,13 +2085,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B93">
-        <v>427211.63491899997</v>
+        <v>427199.387766</v>
       </c>
       <c r="C93">
-        <v>6654950.92655</v>
+        <v>6654953.6541600004</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -2096,13 +2099,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B94">
-        <v>427218.57246400003</v>
+        <v>427211.63491899997</v>
       </c>
       <c r="C94">
-        <v>6654949.0793199996</v>
+        <v>6654950.92655</v>
       </c>
       <c r="D94">
         <v>2</v>
@@ -2110,27 +2113,27 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="B95">
-        <v>426918.37400000001</v>
+        <v>427218.57246400003</v>
       </c>
       <c r="C95">
-        <v>6654803.2980000004</v>
+        <v>6654949.0793199996</v>
       </c>
       <c r="D95">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="B96">
-        <v>427074.70942299999</v>
+        <v>426918.37400000001</v>
       </c>
       <c r="C96">
-        <v>6654805.1742099999</v>
+        <v>6654803.2980000004</v>
       </c>
       <c r="D96">
         <v>3</v>
@@ -2138,13 +2141,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B97">
-        <v>427409.54730099998</v>
+        <v>427074.70942299999</v>
       </c>
       <c r="C97">
-        <v>6655023.2711699996</v>
+        <v>6654805.1742099999</v>
       </c>
       <c r="D97">
         <v>3</v>
@@ -2152,13 +2155,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B98">
-        <v>427473.89030299999</v>
+        <v>427409.54730099998</v>
       </c>
       <c r="C98">
-        <v>6655012.0804500002</v>
+        <v>6655023.2711699996</v>
       </c>
       <c r="D98">
         <v>3</v>
@@ -2166,13 +2169,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B99">
-        <v>427454.97677200002</v>
+        <v>427473.89030299999</v>
       </c>
       <c r="C99">
-        <v>6655155.6970300004</v>
+        <v>6655012.0804500002</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -2180,13 +2183,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B100">
-        <v>427448.93046300003</v>
+        <v>427454.97677200002</v>
       </c>
       <c r="C100">
-        <v>6655144.2890999997</v>
+        <v>6655155.6970300004</v>
       </c>
       <c r="D100">
         <v>3</v>
@@ -2194,13 +2197,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B101">
-        <v>427384.17204400001</v>
+        <v>427448.93046300003</v>
       </c>
       <c r="C101">
-        <v>6655037.1886999998</v>
+        <v>6655144.2890999997</v>
       </c>
       <c r="D101">
         <v>3</v>
@@ -2208,13 +2211,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B102">
-        <v>427353.18437899998</v>
+        <v>427384.17204400001</v>
       </c>
       <c r="C102">
-        <v>6655078.9283299996</v>
+        <v>6655037.1886999998</v>
       </c>
       <c r="D102">
         <v>3</v>
@@ -2222,13 +2225,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B103">
-        <v>427436.22735900001</v>
+        <v>427353.18437899998</v>
       </c>
       <c r="C103">
-        <v>6654995.7281400003</v>
+        <v>6655078.9283299996</v>
       </c>
       <c r="D103">
         <v>3</v>
@@ -2236,13 +2239,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B104">
-        <v>427473.82857299998</v>
+        <v>427436.22735900001</v>
       </c>
       <c r="C104">
-        <v>6655256.9652800001</v>
+        <v>6654995.7281400003</v>
       </c>
       <c r="D104">
         <v>3</v>
@@ -2250,13 +2253,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B105">
-        <v>427162.88967599999</v>
+        <v>427473.82857299998</v>
       </c>
       <c r="C105">
-        <v>6654757.2354899999</v>
+        <v>6655256.9652800001</v>
       </c>
       <c r="D105">
         <v>3</v>
@@ -2264,13 +2267,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B106">
-        <v>427461.85729999997</v>
+        <v>427162.88967599999</v>
       </c>
       <c r="C106">
-        <v>6655153.3641299997</v>
+        <v>6654757.2354899999</v>
       </c>
       <c r="D106">
         <v>3</v>
@@ -2278,13 +2281,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B107">
-        <v>427451.795231</v>
+        <v>427461.85729999997</v>
       </c>
       <c r="C107">
-        <v>6655150.5926099997</v>
+        <v>6655153.3641299997</v>
       </c>
       <c r="D107">
         <v>3</v>
@@ -2292,13 +2295,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B108">
-        <v>427454.58941900003</v>
+        <v>427451.795231</v>
       </c>
       <c r="C108">
-        <v>6655141.5299500003</v>
+        <v>6655150.5926099997</v>
       </c>
       <c r="D108">
         <v>3</v>
@@ -2306,13 +2309,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>144</v>
+        <v>79</v>
       </c>
       <c r="B109">
-        <v>427451.88591100002</v>
+        <v>427454.58941900003</v>
       </c>
       <c r="C109">
-        <v>6655154.5902399998</v>
+        <v>6655141.5299500003</v>
       </c>
       <c r="D109">
         <v>3</v>
@@ -2320,13 +2323,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="B110">
-        <v>427470.63105600001</v>
+        <v>427451.88591100002</v>
       </c>
       <c r="C110">
-        <v>6655011.1764599998</v>
+        <v>6655154.5902399998</v>
       </c>
       <c r="D110">
         <v>3</v>
@@ -2334,13 +2337,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B111">
-        <v>427459.94916800002</v>
+        <v>427470.63105600001</v>
       </c>
       <c r="C111">
-        <v>6655157.4070899999</v>
+        <v>6655011.1764599998</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -2348,13 +2351,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B112">
-        <v>427471.152459</v>
+        <v>427459.94916800002</v>
       </c>
       <c r="C112">
-        <v>6655034.1627900004</v>
+        <v>6655157.4070899999</v>
       </c>
       <c r="D112">
         <v>3</v>
@@ -2362,13 +2365,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B113">
-        <v>427448.77434300003</v>
+        <v>427471.152459</v>
       </c>
       <c r="C113">
-        <v>6655149.6612200001</v>
+        <v>6655034.1627900004</v>
       </c>
       <c r="D113">
         <v>3</v>
@@ -2376,13 +2379,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B114">
-        <v>427437.28213900002</v>
+        <v>427448.77434300003</v>
       </c>
       <c r="C114">
-        <v>6655127.9236500002</v>
+        <v>6655149.6612200001</v>
       </c>
       <c r="D114">
         <v>3</v>
@@ -2390,13 +2393,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B115">
-        <v>427428.46884500002</v>
+        <v>427437.28213900002</v>
       </c>
       <c r="C115">
-        <v>6655136.1229299996</v>
+        <v>6655127.9236500002</v>
       </c>
       <c r="D115">
         <v>3</v>
@@ -2404,13 +2407,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B116">
-        <v>427449.97970800003</v>
+        <v>427428.46884500002</v>
       </c>
       <c r="C116">
-        <v>6655114.6366699999</v>
+        <v>6655136.1229299996</v>
       </c>
       <c r="D116">
         <v>3</v>
@@ -2418,13 +2421,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B117">
-        <v>427463.33470299997</v>
+        <v>427449.97970800003</v>
       </c>
       <c r="C117">
-        <v>6655130.3324499996</v>
+        <v>6655114.6366699999</v>
       </c>
       <c r="D117">
         <v>3</v>
@@ -2432,13 +2435,13 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B118">
-        <v>427464.67415799998</v>
+        <v>427463.33470299997</v>
       </c>
       <c r="C118">
-        <v>6655145.3008700004</v>
+        <v>6655130.3324499996</v>
       </c>
       <c r="D118">
         <v>3</v>
@@ -2446,13 +2449,13 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B119">
-        <v>427463.52186600002</v>
+        <v>427464.67415799998</v>
       </c>
       <c r="C119">
-        <v>6655006.3381099999</v>
+        <v>6655145.3008700004</v>
       </c>
       <c r="D119">
         <v>3</v>
@@ -2460,13 +2463,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B120">
-        <v>427456.07263200002</v>
+        <v>427463.52186600002</v>
       </c>
       <c r="C120">
-        <v>6654986.50868</v>
+        <v>6655006.3381099999</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -2474,13 +2477,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B121">
-        <v>427363.30535500002</v>
+        <v>427456.07263200002</v>
       </c>
       <c r="C121">
-        <v>6655084.6052799998</v>
+        <v>6654986.50868</v>
       </c>
       <c r="D121">
         <v>3</v>
@@ -2488,13 +2491,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B122">
-        <v>427443.730048</v>
+        <v>427363.30535500002</v>
       </c>
       <c r="C122">
-        <v>6655191.7722899998</v>
+        <v>6655084.6052799998</v>
       </c>
       <c r="D122">
         <v>3</v>
@@ -2502,13 +2505,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B123">
-        <v>427449.771824</v>
+        <v>427443.730048</v>
       </c>
       <c r="C123">
-        <v>6655193.6350800004</v>
+        <v>6655191.7722899998</v>
       </c>
       <c r="D123">
         <v>3</v>
@@ -2516,13 +2519,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B124">
-        <v>427453.49740699999</v>
+        <v>427449.771824</v>
       </c>
       <c r="C124">
-        <v>6655181.5515299998</v>
+        <v>6655193.6350800004</v>
       </c>
       <c r="D124">
         <v>3</v>
@@ -2530,13 +2533,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B125">
-        <v>427443.16329699999</v>
+        <v>427453.49740699999</v>
       </c>
       <c r="C125">
-        <v>6655166.7871399997</v>
+        <v>6655181.5515299998</v>
       </c>
       <c r="D125">
         <v>3</v>
@@ -2544,13 +2547,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B126">
-        <v>427445.95748500002</v>
+        <v>427443.16329699999</v>
       </c>
       <c r="C126">
-        <v>6655157.7244699998</v>
+        <v>6655166.7871399997</v>
       </c>
       <c r="D126">
         <v>3</v>
@@ -2558,13 +2561,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B127">
-        <v>427419.01886399998</v>
+        <v>427445.95748500002</v>
       </c>
       <c r="C127">
-        <v>6655160.3353700005</v>
+        <v>6655157.7244699998</v>
       </c>
       <c r="D127">
         <v>3</v>
@@ -2572,13 +2575,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B128">
-        <v>427409.62389599998</v>
+        <v>427419.01886399998</v>
       </c>
       <c r="C128">
-        <v>6654966.5639599999</v>
+        <v>6655160.3353700005</v>
       </c>
       <c r="D128">
         <v>3</v>
@@ -2586,13 +2589,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B129">
-        <v>427348.77541900001</v>
+        <v>427409.62389599998</v>
       </c>
       <c r="C129">
-        <v>6654928.9473000001</v>
+        <v>6654966.5639599999</v>
       </c>
       <c r="D129">
         <v>3</v>
@@ -2600,13 +2603,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B130">
-        <v>427358.29147300002</v>
+        <v>427348.77541900001</v>
       </c>
       <c r="C130">
-        <v>6654951.7296099998</v>
+        <v>6654928.9473000001</v>
       </c>
       <c r="D130">
         <v>3</v>
@@ -2614,13 +2617,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B131">
-        <v>427459.27487700002</v>
+        <v>427358.29147300002</v>
       </c>
       <c r="C131">
-        <v>6654995.4353299998</v>
+        <v>6654951.7296099998</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -2628,13 +2631,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>147</v>
+        <v>26</v>
       </c>
       <c r="B132">
-        <v>427474.83270700002</v>
+        <v>427459.27487700002</v>
       </c>
       <c r="C132">
-        <v>6655020.0804300001</v>
+        <v>6654995.4353299998</v>
       </c>
       <c r="D132">
         <v>3</v>
@@ -2642,13 +2645,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="B133">
-        <v>427309.979934</v>
+        <v>427474.83270700002</v>
       </c>
       <c r="C133">
-        <v>6654937.8266599998</v>
+        <v>6655020.0804300001</v>
       </c>
       <c r="D133">
         <v>3</v>
@@ -2656,13 +2659,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B134">
-        <v>427397.49695300002</v>
+        <v>427309.979934</v>
       </c>
       <c r="C134">
-        <v>6654916.8430199996</v>
+        <v>6654937.8266599998</v>
       </c>
       <c r="D134">
         <v>3</v>
@@ -2670,13 +2673,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B135">
-        <v>427394.22670100001</v>
+        <v>427397.49695300002</v>
       </c>
       <c r="C135">
-        <v>6654904.9181599999</v>
+        <v>6654916.8430199996</v>
       </c>
       <c r="D135">
         <v>3</v>
@@ -2684,13 +2687,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B136">
-        <v>427400.33648499998</v>
+        <v>427394.22670100001</v>
       </c>
       <c r="C136">
-        <v>6654909.77917</v>
+        <v>6654904.9181599999</v>
       </c>
       <c r="D136">
         <v>3</v>
@@ -2698,13 +2701,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B137">
-        <v>427372.48913200002</v>
+        <v>427400.33648499998</v>
       </c>
       <c r="C137">
-        <v>6654916.4103499996</v>
+        <v>6654909.77917</v>
       </c>
       <c r="D137">
         <v>3</v>
@@ -2712,13 +2715,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B138">
-        <v>427393.15733900003</v>
+        <v>427372.48913200002</v>
       </c>
       <c r="C138">
-        <v>6654945.93915</v>
+        <v>6654916.4103499996</v>
       </c>
       <c r="D138">
         <v>3</v>
@@ -2726,13 +2729,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B139">
-        <v>427387.342259</v>
+        <v>427393.15733900003</v>
       </c>
       <c r="C139">
-        <v>6654954.0704100002</v>
+        <v>6654945.93915</v>
       </c>
       <c r="D139">
         <v>3</v>
@@ -2740,13 +2743,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B140">
-        <v>427191.59464899998</v>
+        <v>427387.342259</v>
       </c>
       <c r="C140">
-        <v>6654964.51009</v>
+        <v>6654954.0704100002</v>
       </c>
       <c r="D140">
         <v>3</v>
@@ -2754,13 +2757,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>135</v>
+        <v>9</v>
       </c>
       <c r="B141">
-        <v>427215.44438599999</v>
+        <v>427191.59464899998</v>
       </c>
       <c r="C141">
-        <v>6654957.9695800003</v>
+        <v>6654964.51009</v>
       </c>
       <c r="D141">
         <v>3</v>
@@ -2768,13 +2771,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>6</v>
+        <v>135</v>
       </c>
       <c r="B142">
-        <v>427250.03822699998</v>
+        <v>427215.44438599999</v>
       </c>
       <c r="C142">
-        <v>6654940.1862300001</v>
+        <v>6654957.9695800003</v>
       </c>
       <c r="D142">
         <v>3</v>
@@ -2782,13 +2785,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B143">
-        <v>427229.09603199997</v>
+        <v>427250.03822699998</v>
       </c>
       <c r="C143">
-        <v>6654942.6611099998</v>
+        <v>6654940.1862300001</v>
       </c>
       <c r="D143">
         <v>3</v>
@@ -2796,13 +2799,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B144">
-        <v>427447.87335800001</v>
+        <v>427229.09603199997</v>
       </c>
       <c r="C144">
-        <v>6654977.69539</v>
+        <v>6654942.6611099998</v>
       </c>
       <c r="D144">
         <v>3</v>
@@ -2810,15 +2813,29 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B145">
+        <v>427447.87335800001</v>
+      </c>
+      <c r="C145">
+        <v>6654977.69539</v>
+      </c>
+      <c r="D145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146">
         <v>427468.74921799998</v>
       </c>
-      <c r="C145">
+      <c r="C146">
         <v>6654985.5211899998</v>
       </c>
-      <c r="D145">
+      <c r="D146">
         <v>3</v>
       </c>
     </row>

</xml_diff>